<commit_message>
Dashboard test case updated with real data.
</commit_message>
<xml_diff>
--- a/Tests/Test Cases/dashboard.xlsx
+++ b/Tests/Test Cases/dashboard.xlsx
@@ -5,11 +5,11 @@
   <workbookPr filterPrivacy="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tthakgunduz/Desktop/SWE574/GiTHUB/docs-repo/Tests/Test Cases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tthakgunduz/Desktop/ALL/Master-BOUN/SWE574/GiTHUB/docs-repo/Tests/Test Cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="3820" windowWidth="24000" windowHeight="13560"/>
+    <workbookView xWindow="440" yWindow="4800" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Task Name</t>
   </si>
@@ -56,12 +56,6 @@
     <t>User opens http://localhost:8080/dashboard.html?uid=x page.</t>
   </si>
   <si>
-    <t>1- Login to application on index.html page</t>
-  </si>
-  <si>
-    <t>Dashboard page is opened with the user's communities.</t>
-  </si>
-  <si>
     <t>#179, #180</t>
   </si>
   <si>
@@ -71,18 +65,9 @@
     <t>1- Click on My Profile menu.</t>
   </si>
   <si>
-    <t>EditProfile page is opened with user data.</t>
-  </si>
-  <si>
     <t>User opens communities page and joins to an existing community.</t>
   </si>
   <si>
-    <t>1- Click on Communities
-2- Join to an existing community.
-3- Text explanation and click on Send request.
-4- Community owner approves the request.</t>
-  </si>
-  <si>
     <t>User becomes member.</t>
   </si>
   <si>
@@ -95,10 +80,6 @@
     <t>User creates a new community</t>
   </si>
   <si>
-    <t>1- Click on create community
-2- Enter data and click on create.</t>
-  </si>
-  <si>
     <t>Community is crated</t>
   </si>
   <si>
@@ -108,19 +89,7 @@
     <t>4 more community is listed.</t>
   </si>
   <si>
-    <t>1- Open main page.
-2- Click on See More button</t>
-  </si>
-  <si>
     <t>User searches community.</t>
-  </si>
-  <si>
-    <t>Community section is updated with results.</t>
-  </si>
-  <si>
-    <t>1- Open main page.
-2- Enter keyword in search field.
-3- Press enter or click on search button</t>
   </si>
   <si>
     <t>User sorts the communities by Title</t>
@@ -156,18 +125,62 @@
     <t>User displays the communities having a popular group tag.</t>
   </si>
   <si>
+    <t>User views community details.</t>
+  </si>
+  <si>
+    <t>1- Login to application on index.html page with below data:
+emre.gurer@gmail.com
+123</t>
+  </si>
+  <si>
+    <t>Dashboard page is opened with the below communities:
+Sustainable Web Design.</t>
+  </si>
+  <si>
+    <t>EditProfile page is opened with user data.
+Education: MS, Profession: Software Engineering.</t>
+  </si>
+  <si>
+    <t>1- Click on Communities
+2- Join to "Web Community".
+3- Text explanation as "Please approve my request" and click on Send request.
+4- Community owner approves the request.</t>
+  </si>
+  <si>
+    <t>1- Click on create community
+2- Enter title Mobile Developers
+3- Description: Mobile Developers' meeting point
+4-Tags: Mobile, Development
+5- Visibility: Public
+6-Requires Approval: No
+7-Remaining 4 question is All Joined Members
+8-Click on create.</t>
+  </si>
+  <si>
+    <t>1- Open dashbord page.
+2- Click on See More button</t>
+  </si>
+  <si>
+    <t>1- Open dashboard page.
+2- Enter "html" keyword in search field.
+3- Press enter or click on search button</t>
+  </si>
+  <si>
+    <t>Community section is updated with results having html keyword in it.</t>
+  </si>
+  <si>
     <t>1- Open main page.
-2- Click on a popular group tag.</t>
-  </si>
-  <si>
-    <t>User views community details.</t>
-  </si>
-  <si>
-    <t>Community details page is opened.</t>
+2- Click on "html" popular group tag.</t>
+  </si>
+  <si>
+    <t>Community section is updated with results having html group tag.</t>
   </si>
   <si>
     <t>1- Open main page.
-2- Click on community details button on one of community.</t>
+2- Click on community details button on "Web Sustainability".</t>
+  </si>
+  <si>
+    <t>"Web Sustainability" details page is opened.</t>
   </si>
 </sst>
 </file>
@@ -662,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:D13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -708,7 +721,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -716,30 +729,30 @@
         <v>8</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="E3" s="8"/>
       <c r="F3" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="9"/>
@@ -751,37 +764,37 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="150" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -791,13 +804,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="9"/>
@@ -809,13 +822,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="9"/>
@@ -827,13 +840,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="9"/>
@@ -845,13 +858,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="9"/>
@@ -863,13 +876,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="9"/>
@@ -881,13 +894,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="9"/>
@@ -899,10 +912,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>42</v>

</xml_diff>